<commit_message>
Review study and make suggestions
</commit_message>
<xml_diff>
--- a/GaussCalcsCH4.xlsx
+++ b/GaussCalcsCH4.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21320"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokeeffe\1D\Field studies\Methane tracer study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="11_0D4F1271D7DCFD24D6143BF107300E44183D91C1" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0EA18708-8C6F-4061-9D11-A1B5DC8F1FF7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Chart2" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,9 +62,6 @@
   </si>
   <si>
     <t>m stack dia</t>
-  </si>
-  <si>
-    <t>minutes/tank (using critical orifice)</t>
   </si>
   <si>
     <t>vs</t>
@@ -206,12 +202,6 @@
     <t>Limit &lt;5% for safety sake (lower explosive limit) = 0.8 lpm</t>
   </si>
   <si>
-    <t>Best range?:</t>
-  </si>
-  <si>
-    <t>0-1 SLPM highlighted</t>
-  </si>
-  <si>
     <t>CH4 (%)</t>
   </si>
   <si>
@@ -222,12 +212,6 @@
   </si>
   <si>
     <t>Q (sccm)</t>
-  </si>
-  <si>
-    <t>5 cm</t>
-  </si>
-  <si>
-    <t>30 m</t>
   </si>
   <si>
     <t>CH4</t>
@@ -247,18 +231,33 @@
   <si>
     <t>Dilution</t>
   </si>
+  <si>
+    <t>Recommended operating range highlighted</t>
+  </si>
+  <si>
+    <t>@ 5 cm</t>
+  </si>
+  <si>
+    <t>@ 30 m</t>
+  </si>
+  <si>
+    <t>minutes/tank</t>
+  </si>
+  <si>
+    <t>runtime (min)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,12 +307,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -339,6 +337,8 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,88 +769,88 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>1060952.892111443</c:v>
+                  <c:v>3536509.6403714763</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>988404.47793193697</c:v>
+                  <c:v>3294681.5931064566</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>910759.62533433666</c:v>
+                  <c:v>3035865.417781122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>829087.80463930836</c:v>
+                  <c:v>2763626.0154643613</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>744799.66855187982</c:v>
+                  <c:v>2482665.5618395992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>659588.51346557308</c:v>
+                  <c:v>2198628.3782185768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>575325.58774876886</c:v>
+                  <c:v>1917751.9591625629</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>493917.73970429343</c:v>
+                  <c:v>1646392.465680978</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>417146.26402165875</c:v>
+                  <c:v>1390487.5467388625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>346512.96229872917</c:v>
+                  <c:v>1155043.2076624306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>283120.22006291401</c:v>
+                  <c:v>943734.06687638001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7837.5958810188913</c:v>
+                  <c:v>26125.319603396303</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5572.8897068674087</c:v>
+                  <c:v>18576.299022891362</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3947.8585171310674</c:v>
+                  <c:v>13159.528390436892</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2787.8435706250098</c:v>
+                  <c:v>9292.8119020833656</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1963.4077097818313</c:v>
+                  <c:v>6544.692365939437</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1379.647480822545</c:v>
+                  <c:v>4598.8249360751497</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>967.59940878027351</c:v>
+                  <c:v>3225.3313626009117</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>677.52343347499345</c:v>
+                  <c:v>2258.411444916645</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>473.76818683144052</c:v>
+                  <c:v>1579.2272894381351</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>330.91370362625202</c:v>
+                  <c:v>1103.0456787541734</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>230.91418506953752</c:v>
+                  <c:v>769.71395023179184</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>161.00546911884567</c:v>
+                  <c:v>536.68489706281889</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>112.18675653547345</c:v>
+                  <c:v>373.95585511824487</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>89.349251564576122</c:v>
+                  <c:v>297.83083854858705</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>62.228213190723018</c:v>
+                  <c:v>207.42737730241006</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43.475066965412189</c:v>
+                  <c:v>144.9168898847073</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>30.797496506763565</c:v>
+                  <c:v>102.65832168921189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,11 +1293,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2072,11 +2067,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3193,10 +3183,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3204,10 +3194,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4046,51 +4036,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19">
+      <c r="D1" s="18">
         <f>B1/16*60*25</f>
-        <v>2.8124999999999997E-2</v>
+        <v>9.375E-2</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="7"/>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1">
         <f>B1/454*60</f>
-        <v>3.9647577092511014E-5</v>
+        <v>1.3215859030837003E-4</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4107,7 +4097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4118,269 +4108,269 @@
         <v>9</v>
       </c>
       <c r="F3" s="2">
-        <f>(F2*0.48)/D1</f>
-        <v>955.73333333333335</v>
+        <f>F2/D1</f>
+        <v>597.33333333333337</v>
       </c>
       <c r="G3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>13</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
         <v>14</v>
       </c>
-      <c r="N5" t="s">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
-        <v>16</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <f>B6*3.14159/180</f>
         <v>0.13962622222222221</v>
       </c>
       <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
         <v>18</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>19</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>21</v>
       </c>
-      <c r="R6" t="s">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>23</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f>B7*3.14159/180</f>
         <v>0.13962622222222221</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" t="s">
         <v>24</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>25</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>27</v>
       </c>
-      <c r="R7" t="s">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
-        <v>29</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="O8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="P8" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="Q8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="R8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="R8" s="21" t="s">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
       <c r="B9">
         <v>0.1</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <f>B9^0.5</f>
         <v>0.31622776601683794</v>
       </c>
       <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" t="s">
         <v>37</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>39</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>40</v>
       </c>
-      <c r="R9" t="s">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
-        <v>42</v>
       </c>
       <c r="B10">
         <f>(1/4-1/8)*2.54/100</f>
         <v>3.1749999999999999E-3</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="N10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" t="s">
         <v>44</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>45</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>46</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>47</v>
       </c>
-      <c r="R10" t="s">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="13" t="s">
+      <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="G11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="14">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>0.05</v>
       </c>
       <c r="B12" s="1">
         <f>1.44*((B$4*B$3)^0.667)*(A12^0.333)/(B$2^0.6667)+B$5</f>
         <v>1</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>A12*D$6*$B$9+$B$10</f>
         <v>3.8731311111111109E-3</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <f>A12*D$7*$B$9+$B$10</f>
         <v>3.8731311111111109E-3</v>
       </c>
       <c r="E12" s="1">
         <f>B$1*1000000/(2*3.14159*C12*D12*B$2)*(EXP(-0.5*((B12+B$8)/D12)^2)+EXP(-0.5*((B12-B$8)/D12)^2))</f>
-        <v>1060952.892111443</v>
+        <v>3536509.6403714763</v>
       </c>
       <c r="F12" s="2">
         <f>0.025/16000000*1000000*$E12</f>
-        <v>1657.7388939241298</v>
-      </c>
-      <c r="G12" s="17">
+        <v>5525.7963130804319</v>
+      </c>
+      <c r="G12" s="16">
         <f>0.025/16000000*$E12</f>
-        <v>1.6577388939241298E-3</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>56</v>
+        <v>5.5257963130804326E-3</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="14">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
         <f>1.2*A12</f>
         <v>0.06</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ref="B12:B22" si="0">1.44*((B$4*B$3)^0.667)*(A13^0.333)/(B$2^0.6667)+B$5</f>
+        <f t="shared" ref="B13:B22" si="0">1.44*((B$4*B$3)^0.667)*(A13^0.333)/(B$2^0.6667)+B$5</f>
         <v>1</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <f t="shared" ref="C13:C22" si="1">A13*D$6*$B$9+$B$10</f>
         <v>4.0127573333333336E-3</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <f t="shared" ref="D13:D22" si="2">A13*D$7*$B$9+$B$10</f>
         <v>4.0127573333333336E-3</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ref="E13:E22" si="3">B$1*1000000/(2*3.14159*C13*D13*B$2)*(EXP(-0.5*((B13+B$8)/D13)^2)+EXP(-0.5*((B13-B$8)/D13)^2))</f>
-        <v>988404.47793193697</v>
+        <v>3294681.5931064566</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" ref="F13:F22" si="4">0.025/16000000*1000000*E13</f>
-        <v>1544.3819967686516</v>
-      </c>
-      <c r="G13" s="17">
+        <v>5147.9399892288384</v>
+      </c>
+      <c r="G13" s="16">
         <f t="shared" ref="G13:G22" si="5">0.025/16000000*$E13</f>
-        <v>1.5443819967686516E-3</v>
+        <v>5.1479399892288384E-3</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -4388,8 +4378,8 @@
       <c r="N13" s="1"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="14">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <f t="shared" ref="A14:A22" si="6">1.2*A13</f>
         <v>7.1999999999999995E-2</v>
       </c>
@@ -4397,36 +4387,33 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f t="shared" si="1"/>
         <v>4.1803088E-3</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <f t="shared" si="2"/>
         <v>4.1803088E-3</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="3"/>
-        <v>910759.62533433666</v>
+        <v>3035865.417781122</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="4"/>
-        <v>1423.0619145849012</v>
-      </c>
-      <c r="G14" s="17">
+        <v>4743.5397152830037</v>
+      </c>
+      <c r="G14" s="16">
         <f t="shared" si="5"/>
-        <v>1.4230619145849011E-3</v>
+        <v>4.7435397152830036E-3</v>
       </c>
       <c r="K14" s="1"/>
-      <c r="L14" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="14">
+      <c r="L14" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
         <f t="shared" si="6"/>
         <v>8.6399999999999991E-2</v>
       </c>
@@ -4434,38 +4421,38 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <f t="shared" si="1"/>
         <v>4.3813705599999994E-3</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f t="shared" si="2"/>
         <v>4.3813705599999994E-3</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="3"/>
-        <v>829087.80463930836</v>
+        <v>2763626.0154643613</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="4"/>
-        <v>1295.4496947489195</v>
-      </c>
-      <c r="G15" s="17">
+        <v>4318.1656491630647</v>
+      </c>
+      <c r="G15" s="16">
         <f t="shared" si="5"/>
-        <v>1.2954496947489194E-3</v>
+        <v>4.318165649163065E-3</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <f t="shared" si="6"/>
         <v>0.10367999999999998</v>
       </c>
@@ -4473,42 +4460,45 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <f t="shared" si="1"/>
         <v>4.6226446719999995E-3</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <f t="shared" si="2"/>
         <v>4.6226446719999995E-3</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="3"/>
-        <v>744799.66855187982</v>
+        <v>2482665.5618395992</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="4"/>
-        <v>1163.7494821123123</v>
-      </c>
-      <c r="G16" s="17">
+        <v>3879.1649403743741</v>
+      </c>
+      <c r="G16" s="16">
         <f>0.025/16000000*$E16</f>
-        <v>1.1637494821123123E-3</v>
+        <v>3.8791649403743739E-3</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="14">
+        <v>59</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="P16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <f t="shared" si="6"/>
         <v>0.12441599999999997</v>
       </c>
@@ -4516,28 +4506,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <f t="shared" si="1"/>
         <v>4.9121736063999994E-3</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <f t="shared" si="2"/>
         <v>4.9121736063999994E-3</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="3"/>
-        <v>659588.51346557308</v>
+        <v>2198628.3782185768</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="4"/>
-        <v>1030.6070522899579</v>
-      </c>
-      <c r="G17" s="17">
+        <v>3435.3568409665263</v>
+      </c>
+      <c r="G17" s="16">
         <f t="shared" si="5"/>
-        <v>1.030607052289958E-3</v>
+        <v>3.4353568409665265E-3</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="10">
+      <c r="L17" s="9">
         <v>1E-4</v>
       </c>
       <c r="M17">
@@ -4546,12 +4536,16 @@
       <c r="N17" s="2">
         <v>0.1</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="19">
         <v>4.7E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="14">
+      <c r="P17" s="1">
+        <f>$F$2*1000/M17</f>
+        <v>6222.2222222222226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <f>1.2*A17</f>
         <v>0.14929919999999997</v>
       </c>
@@ -4559,42 +4553,46 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <f t="shared" si="1"/>
         <v>5.2596083276799993E-3</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <f t="shared" si="2"/>
         <v>5.2596083276799993E-3</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="3"/>
-        <v>575325.58774876886</v>
+        <v>1917751.9591625629</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="4"/>
-        <v>898.94623085745138</v>
-      </c>
-      <c r="G18" s="17">
+        <v>2996.4874361915045</v>
+      </c>
+      <c r="G18" s="16">
         <f t="shared" si="5"/>
-        <v>8.989462308574514E-4</v>
+        <v>2.9964874361915047E-3</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="M18" s="21">
-        <v>28</v>
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="M18" s="20">
+        <v>42</v>
       </c>
       <c r="N18">
         <v>0.2</v>
       </c>
-      <c r="O18" s="19">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="14">
+      <c r="O18" s="18">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" ref="P18:P27" si="7">$F$2*1000/M18</f>
+        <v>1333.3333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <f t="shared" si="6"/>
         <v>0.17915903999999996</v>
       </c>
@@ -4602,42 +4600,46 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <f t="shared" si="1"/>
         <v>5.6765299932159995E-3</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <f t="shared" si="2"/>
         <v>5.6765299932159995E-3</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="3"/>
-        <v>493917.73970429343</v>
+        <v>1646392.465680978</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="4"/>
-        <v>771.74646828795858</v>
-      </c>
-      <c r="G19" s="17">
+        <v>2572.4882276265284</v>
+      </c>
+      <c r="G19" s="16">
         <f t="shared" si="5"/>
-        <v>7.7174646828795856E-4</v>
+        <v>2.5724882276265282E-3</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="10">
+      <c r="L19" s="9">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="20">
         <v>47</v>
       </c>
       <c r="N19" s="2">
         <v>0.3</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="18">
         <v>0.23300000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="14">
+      <c r="P19" s="1">
+        <f t="shared" si="7"/>
+        <v>1191.4893617021276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <f t="shared" si="6"/>
         <v>0.21499084799999996</v>
       </c>
@@ -4645,42 +4647,46 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f t="shared" si="1"/>
         <v>6.1768359918591993E-3</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <f t="shared" si="2"/>
         <v>6.1768359918591993E-3</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="3"/>
-        <v>417146.26402165875</v>
+        <v>1390487.5467388625</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="4"/>
-        <v>651.79103753384186</v>
-      </c>
-      <c r="G20" s="17">
+        <v>2172.6367917794728</v>
+      </c>
+      <c r="G20" s="16">
         <f t="shared" si="5"/>
-        <v>6.517910375338419E-4</v>
+        <v>2.1726367917794731E-3</v>
       </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="20">
         <v>66</v>
       </c>
       <c r="N20" s="2">
         <v>0.4</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="18">
         <v>0.32600000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="14">
+      <c r="P20" s="1">
+        <f t="shared" si="7"/>
+        <v>848.4848484848485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <f t="shared" si="6"/>
         <v>0.25798901759999993</v>
       </c>
@@ -4688,42 +4694,46 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <f t="shared" si="1"/>
         <v>6.7772031902310391E-3</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <f t="shared" si="2"/>
         <v>6.7772031902310391E-3</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="3"/>
-        <v>346512.96229872917</v>
+        <v>1155043.2076624306</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="4"/>
-        <v>541.42650359176434</v>
-      </c>
-      <c r="G21" s="17">
+        <v>1804.7550119725479</v>
+      </c>
+      <c r="G21" s="16">
         <f t="shared" si="5"/>
-        <v>5.4142650359176433E-4</v>
+        <v>1.8047550119725479E-3</v>
       </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="19">
+      <c r="L21" s="18">
         <v>1E-3</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="20">
         <v>94</v>
       </c>
       <c r="N21" s="2">
         <v>0.6</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="18">
         <v>0.46500000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="14">
+      <c r="P21" s="1">
+        <f t="shared" si="7"/>
+        <v>595.74468085106378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <f t="shared" si="6"/>
         <v>0.30958682111999991</v>
       </c>
@@ -4731,596 +4741,619 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <f t="shared" si="1"/>
         <v>7.4976438282772463E-3</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <f t="shared" si="2"/>
         <v>7.4976438282772463E-3</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="3"/>
-        <v>283120.22006291401</v>
+        <v>943734.06687638001</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="4"/>
-        <v>442.37534384830315</v>
-      </c>
-      <c r="G22" s="17">
+        <v>1474.5844794943439</v>
+      </c>
+      <c r="G22" s="16">
         <f t="shared" si="5"/>
-        <v>4.4237534384830319E-4</v>
+        <v>1.4745844794943439E-3</v>
       </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="19">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M22" s="21">
-        <v>281</v>
+      <c r="L22" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M22" s="20">
+        <v>469</v>
       </c>
       <c r="N22" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="O22" s="8">
-        <v>1.3959999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="O22" s="7">
+        <v>2.327</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="7"/>
+        <v>119.40298507462687</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
         <v>3</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" ref="B23:B39" si="7">1.44*((B$4*B$3)^0.667)*(A23^0.333)/(B$2^0.6667)+B$5</f>
+        <f t="shared" ref="B23:B39" si="8">1.44*((B$4*B$3)^0.667)*(A23^0.333)/(B$2^0.6667)+B$5</f>
         <v>1</v>
       </c>
-      <c r="C23" s="10">
-        <f t="shared" ref="C23:C39" si="8">A23*D$6*$B$9+$B$10</f>
+      <c r="C23" s="9">
+        <f t="shared" ref="C23:C39" si="9">A23*D$6*$B$9+$B$10</f>
         <v>4.5062866666666659E-2</v>
       </c>
-      <c r="D23" s="10">
-        <f t="shared" ref="D23:D39" si="9">A23*D$7*$B$9+$B$10</f>
+      <c r="D23" s="9">
+        <f t="shared" ref="D23:D39" si="10">A23*D$7*$B$9+$B$10</f>
         <v>4.5062866666666659E-2</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23:E39" si="10">B$1*1000000/(2*3.14159*C23*D23*B$2)*(EXP(-0.5*((B23+B$8)/D23)^2)+EXP(-0.5*((B23-B$8)/D23)^2))</f>
-        <v>7837.5958810188913</v>
+        <f t="shared" ref="E23:E39" si="11">B$1*1000000/(2*3.14159*C23*D23*B$2)*(EXP(-0.5*((B23+B$8)/D23)^2)+EXP(-0.5*((B23-B$8)/D23)^2))</f>
+        <v>26125.319603396303</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" ref="F23:F39" si="11">0.025/16000000*1000000*E23</f>
-        <v>12.246243564092019</v>
-      </c>
-      <c r="G23" s="9"/>
+        <f t="shared" ref="F23:F39" si="12">0.025/16000000*1000000*E23</f>
+        <v>40.820811880306728</v>
+      </c>
+      <c r="G23" s="8"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="19">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="M23" s="21">
-        <v>469</v>
+      <c r="L23" s="9">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="M23" s="20">
+        <v>797</v>
       </c>
       <c r="N23" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="O23" s="8">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="16">
+        <v>4.7</v>
+      </c>
+      <c r="O23" s="7">
+        <v>3.956</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="7"/>
+        <v>70.26348808030113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
         <f>1.2*A23</f>
         <v>3.5999999999999996</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C24" s="10">
-        <f t="shared" si="8"/>
-        <v>5.3440439999999992E-2</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="C24" s="9">
         <f t="shared" si="9"/>
         <v>5.3440439999999992E-2</v>
       </c>
+      <c r="D24" s="9">
+        <f t="shared" si="10"/>
+        <v>5.3440439999999992E-2</v>
+      </c>
       <c r="E24" s="1">
-        <f t="shared" si="10"/>
-        <v>5572.8897068674087</v>
+        <f t="shared" si="11"/>
+        <v>18576.299022891362</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="11"/>
-        <v>8.7076401669803261</v>
-      </c>
-      <c r="G24" s="9"/>
+        <f t="shared" si="12"/>
+        <v>29.025467223267754</v>
+      </c>
+      <c r="G24" s="8"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="19">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="M24" s="21">
+      <c r="L24" s="18">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="M24" s="11">
         <v>844</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="6">
         <v>5</v>
       </c>
-      <c r="O24" s="8">
+      <c r="O24" s="7">
         <v>4.1879999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="16">
-        <f t="shared" ref="A25:A34" si="12">1.2*A24</f>
+      <c r="P24" s="1">
+        <f t="shared" si="7"/>
+        <v>66.350710900473928</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <f t="shared" ref="A25:A34" si="13">1.2*A24</f>
         <v>4.3199999999999994</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C25" s="10">
-        <f t="shared" si="8"/>
-        <v>6.349352799999998E-2</v>
-      </c>
-      <c r="D25" s="10">
+      <c r="C25" s="9">
         <f t="shared" si="9"/>
         <v>6.349352799999998E-2</v>
       </c>
+      <c r="D25" s="9">
+        <f t="shared" si="10"/>
+        <v>6.349352799999998E-2</v>
+      </c>
       <c r="E25" s="1">
-        <f t="shared" si="10"/>
-        <v>3947.8585171310674</v>
+        <f t="shared" si="11"/>
+        <v>13159.528390436892</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="11"/>
-        <v>6.168528933017293</v>
-      </c>
-      <c r="G25" s="9"/>
+        <f t="shared" si="12"/>
+        <v>20.561763110057644</v>
+      </c>
+      <c r="G25" s="8"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="8">
+      <c r="L25" s="7">
         <v>0.01</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="11">
         <v>938</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="6">
         <v>5.5</v>
       </c>
-      <c r="O25" s="8">
+      <c r="O25" s="7">
         <v>4.6500000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="16">
-        <f t="shared" si="12"/>
+      <c r="P25" s="1">
+        <f t="shared" si="7"/>
+        <v>59.701492537313435</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <f t="shared" si="13"/>
         <v>5.1839999999999993</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C26" s="10">
-        <f t="shared" si="8"/>
-        <v>7.5557233599999982E-2</v>
-      </c>
-      <c r="D26" s="10">
+      <c r="C26" s="9">
         <f t="shared" si="9"/>
         <v>7.5557233599999982E-2</v>
       </c>
+      <c r="D26" s="9">
+        <f t="shared" si="10"/>
+        <v>7.5557233599999982E-2</v>
+      </c>
       <c r="E26" s="1">
-        <f t="shared" si="10"/>
-        <v>2787.8435706250098</v>
+        <f t="shared" si="11"/>
+        <v>9292.8119020833656</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="11"/>
-        <v>4.3560055791015779</v>
-      </c>
-      <c r="G26" s="9"/>
+        <f t="shared" si="12"/>
+        <v>14.52001859700526</v>
+      </c>
+      <c r="G26" s="8"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="8">
+      <c r="L26" s="7">
         <v>0.02</v>
       </c>
       <c r="M26">
-        <v>1.875</v>
-      </c>
-      <c r="N26" s="6">
+        <v>1875</v>
+      </c>
+      <c r="N26" s="5">
         <v>11</v>
       </c>
-      <c r="O26" s="8">
+      <c r="O26" s="7">
         <v>9.3070000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="16">
-        <f t="shared" si="12"/>
+      <c r="P26" s="1">
+        <f t="shared" si="7"/>
+        <v>29.866666666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <f t="shared" si="13"/>
         <v>6.2207999999999988</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C27" s="10">
-        <f t="shared" si="8"/>
-        <v>9.0033680319999976E-2</v>
-      </c>
-      <c r="D27" s="10">
+      <c r="C27" s="9">
         <f t="shared" si="9"/>
         <v>9.0033680319999976E-2</v>
       </c>
+      <c r="D27" s="9">
+        <f t="shared" si="10"/>
+        <v>9.0033680319999976E-2</v>
+      </c>
       <c r="E27" s="1">
-        <f t="shared" si="10"/>
-        <v>1963.4077097818313</v>
+        <f t="shared" si="11"/>
+        <v>6544.692365939437</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="11"/>
-        <v>3.0678245465341116</v>
-      </c>
-      <c r="G27" s="9"/>
+        <f t="shared" si="12"/>
+        <v>10.226081821780371</v>
+      </c>
+      <c r="G27" s="8"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="8">
+      <c r="L27" s="7">
         <v>0.05</v>
       </c>
       <c r="M27">
-        <v>4.6879999999999997</v>
-      </c>
-      <c r="N27" s="6">
+        <v>4688</v>
+      </c>
+      <c r="N27" s="5">
         <v>27.6</v>
       </c>
       <c r="O27" s="2">
         <v>23.268000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="16">
-        <f t="shared" si="12"/>
+      <c r="P27" s="1">
+        <f t="shared" si="7"/>
+        <v>11.945392491467576</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <f t="shared" si="13"/>
         <v>7.4649599999999978</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C28" s="10">
-        <f t="shared" si="8"/>
-        <v>0.10740541638399997</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="C28" s="9">
         <f t="shared" si="9"/>
         <v>0.10740541638399997</v>
       </c>
+      <c r="D28" s="9">
+        <f t="shared" si="10"/>
+        <v>0.10740541638399997</v>
+      </c>
       <c r="E28" s="1">
-        <f t="shared" si="10"/>
-        <v>1379.647480822545</v>
+        <f t="shared" si="11"/>
+        <v>4598.8249360751497</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="11"/>
-        <v>2.1556991887852268</v>
-      </c>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="16">
         <f t="shared" si="12"/>
+        <v>7.1856639626174221</v>
+      </c>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <f t="shared" si="13"/>
         <v>8.957951999999997</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C29" s="10">
-        <f t="shared" si="8"/>
-        <v>0.12825149966079996</v>
-      </c>
-      <c r="D29" s="10">
+      <c r="C29" s="9">
         <f t="shared" si="9"/>
         <v>0.12825149966079996</v>
       </c>
+      <c r="D29" s="9">
+        <f t="shared" si="10"/>
+        <v>0.12825149966079996</v>
+      </c>
       <c r="E29" s="1">
-        <f t="shared" si="10"/>
-        <v>967.59940878027351</v>
+        <f t="shared" si="11"/>
+        <v>3225.3313626009117</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="11"/>
-        <v>1.5118740762191774</v>
-      </c>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="16">
         <f t="shared" si="12"/>
+        <v>5.0395802540639245</v>
+      </c>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <f t="shared" si="13"/>
         <v>10.749542399999996</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C30" s="10">
-        <f t="shared" si="8"/>
-        <v>0.15326679959295994</v>
-      </c>
-      <c r="D30" s="10">
+      <c r="C30" s="9">
         <f t="shared" si="9"/>
         <v>0.15326679959295994</v>
       </c>
+      <c r="D30" s="9">
+        <f t="shared" si="10"/>
+        <v>0.15326679959295994</v>
+      </c>
       <c r="E30" s="1">
-        <f t="shared" si="10"/>
-        <v>677.52343347499345</v>
+        <f t="shared" si="11"/>
+        <v>2258.411444916645</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="11"/>
-        <v>1.0586303648046773</v>
-      </c>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="16">
         <f t="shared" si="12"/>
+        <v>3.5287678826822582</v>
+      </c>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <f t="shared" si="13"/>
         <v>12.899450879999995</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C31" s="10">
-        <f t="shared" si="8"/>
-        <v>0.18328515951155194</v>
-      </c>
-      <c r="D31" s="10">
+      <c r="C31" s="9">
         <f t="shared" si="9"/>
         <v>0.18328515951155194</v>
       </c>
+      <c r="D31" s="9">
+        <f t="shared" si="10"/>
+        <v>0.18328515951155194</v>
+      </c>
       <c r="E31" s="1">
-        <f t="shared" si="10"/>
-        <v>473.76818683144052</v>
+        <f t="shared" si="11"/>
+        <v>1579.2272894381351</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="11"/>
-        <v>0.74026279192412581</v>
-      </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="16">
         <f t="shared" si="12"/>
+        <v>2.4675426397470863</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <f t="shared" si="13"/>
         <v>15.479341055999992</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C32" s="10">
-        <f t="shared" si="8"/>
-        <v>0.21930719141386229</v>
-      </c>
-      <c r="D32" s="10">
+      <c r="C32" s="9">
         <f t="shared" si="9"/>
         <v>0.21930719141386229</v>
       </c>
+      <c r="D32" s="9">
+        <f t="shared" si="10"/>
+        <v>0.21930719141386229</v>
+      </c>
       <c r="E32" s="1">
-        <f t="shared" si="10"/>
-        <v>330.91370362625202</v>
+        <f t="shared" si="11"/>
+        <v>1103.0456787541734</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="11"/>
-        <v>0.51705266191601884</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="16">
         <f t="shared" si="12"/>
+        <v>1.7235088730533961</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <f t="shared" si="13"/>
         <v>18.575209267199991</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C33" s="10">
-        <f t="shared" si="8"/>
-        <v>0.26253362969663474</v>
-      </c>
-      <c r="D33" s="10">
+      <c r="C33" s="9">
         <f t="shared" si="9"/>
         <v>0.26253362969663474</v>
       </c>
+      <c r="D33" s="9">
+        <f t="shared" si="10"/>
+        <v>0.26253362969663474</v>
+      </c>
       <c r="E33" s="1">
-        <f t="shared" si="10"/>
-        <v>230.91418506953752</v>
+        <f t="shared" si="11"/>
+        <v>769.71395023179184</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="11"/>
-        <v>0.36080341417115241</v>
-      </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="16">
         <f t="shared" si="12"/>
+        <v>1.2026780472371748</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <f t="shared" si="13"/>
         <v>22.29025112063999</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C34" s="10">
-        <f t="shared" si="8"/>
-        <v>0.31440535563596167</v>
-      </c>
-      <c r="D34" s="10">
+      <c r="C34" s="9">
         <f t="shared" si="9"/>
         <v>0.31440535563596167</v>
       </c>
+      <c r="D34" s="9">
+        <f t="shared" si="10"/>
+        <v>0.31440535563596167</v>
+      </c>
       <c r="E34" s="1">
-        <f t="shared" si="10"/>
-        <v>161.00546911884567</v>
+        <f t="shared" si="11"/>
+        <v>536.68489706281889</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="11"/>
-        <v>0.25157104549819637</v>
-      </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="16">
+        <f t="shared" si="12"/>
+        <v>0.83857015166065452</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
         <f>1.2*A34</f>
         <v>26.748301344767988</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C35" s="10">
-        <f t="shared" si="8"/>
-        <v>0.37665142676315405</v>
-      </c>
-      <c r="D35" s="10">
+      <c r="C35" s="9">
         <f t="shared" si="9"/>
         <v>0.37665142676315405</v>
       </c>
+      <c r="D35" s="9">
+        <f t="shared" si="10"/>
+        <v>0.37665142676315405</v>
+      </c>
       <c r="E35" s="1">
-        <f t="shared" si="10"/>
-        <v>112.18675653547345</v>
+        <f t="shared" si="11"/>
+        <v>373.95585511824487</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="11"/>
-        <v>0.17529180708667727</v>
-      </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
+        <f t="shared" si="12"/>
+        <v>0.58430602362225759</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="16">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
         <v>30</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C36" s="10">
-        <f t="shared" si="8"/>
-        <v>0.4220536666666666</v>
-      </c>
-      <c r="D36" s="10">
+      <c r="C36" s="9">
         <f t="shared" si="9"/>
         <v>0.4220536666666666</v>
       </c>
+      <c r="D36" s="9">
+        <f t="shared" si="10"/>
+        <v>0.4220536666666666</v>
+      </c>
       <c r="E36" s="1">
-        <f t="shared" si="10"/>
-        <v>89.349251564576122</v>
-      </c>
-      <c r="F36" s="19">
         <f t="shared" si="11"/>
-        <v>0.1396082055696502</v>
-      </c>
-      <c r="G36" s="9"/>
+        <v>297.83083854858705</v>
+      </c>
+      <c r="F36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.46536068523216728</v>
+      </c>
+      <c r="G36" s="8"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="16">
-        <f t="shared" ref="A37:A39" si="13">1.2*A36</f>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <f t="shared" ref="A37:A39" si="14">1.2*A36</f>
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C37" s="10">
-        <f t="shared" si="8"/>
-        <v>0.50582939999999998</v>
-      </c>
-      <c r="D37" s="10">
+      <c r="C37" s="9">
         <f t="shared" si="9"/>
         <v>0.50582939999999998</v>
       </c>
+      <c r="D37" s="9">
+        <f t="shared" si="10"/>
+        <v>0.50582939999999998</v>
+      </c>
       <c r="E37" s="1">
-        <f t="shared" si="10"/>
-        <v>62.228213190723018</v>
+        <f t="shared" si="11"/>
+        <v>207.42737730241006</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="11"/>
-        <v>9.7231583110504727E-2</v>
-      </c>
-      <c r="G37" s="9"/>
+        <f t="shared" si="12"/>
+        <v>0.32410527703501574</v>
+      </c>
+      <c r="G37" s="8"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="16">
-        <f t="shared" si="13"/>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <f t="shared" si="14"/>
         <v>43.199999999999996</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C38" s="10">
-        <f t="shared" si="8"/>
-        <v>0.60636027999999997</v>
-      </c>
-      <c r="D38" s="10">
+      <c r="C38" s="9">
         <f t="shared" si="9"/>
         <v>0.60636027999999997</v>
       </c>
+      <c r="D38" s="9">
+        <f t="shared" si="10"/>
+        <v>0.60636027999999997</v>
+      </c>
       <c r="E38" s="1">
-        <f t="shared" si="10"/>
-        <v>43.475066965412189</v>
+        <f t="shared" si="11"/>
+        <v>144.9168898847073</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="11"/>
-        <v>6.7929792133456554E-2</v>
-      </c>
-      <c r="G38" s="9"/>
+        <f t="shared" si="12"/>
+        <v>0.22643264044485517</v>
+      </c>
+      <c r="G38" s="8"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="16">
-        <f t="shared" si="13"/>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <f t="shared" si="14"/>
         <v>51.839999999999996</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C39" s="10">
-        <f t="shared" si="8"/>
-        <v>0.72699733599999994</v>
-      </c>
-      <c r="D39" s="10">
+      <c r="C39" s="9">
         <f t="shared" si="9"/>
         <v>0.72699733599999994</v>
       </c>
+      <c r="D39" s="9">
+        <f t="shared" si="10"/>
+        <v>0.72699733599999994</v>
+      </c>
       <c r="E39" s="1">
-        <f t="shared" si="10"/>
-        <v>30.797496506763565</v>
+        <f t="shared" si="11"/>
+        <v>102.65832168921189</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="11"/>
-        <v>4.8121088291818076E-2</v>
-      </c>
-      <c r="G39" s="9"/>
+        <f t="shared" si="12"/>
+        <v>0.16040362763939359</v>
+      </c>
+      <c r="G39" s="8"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -5333,7 +5366,7 @@
       <c r="N40" s="1"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -5346,20 +5379,20 @@
       <c r="N41" s="1"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" spans="1:15">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="2"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -5372,7 +5405,7 @@
       <c r="N43" s="1"/>
       <c r="O43" s="2"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -5385,7 +5418,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="2"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5398,7 +5431,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="2"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -5411,7 +5444,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="2"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -5424,7 +5457,7 @@
       <c r="N47" s="1"/>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -5437,7 +5470,7 @@
       <c r="N48" s="1"/>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -5450,7 +5483,7 @@
       <c r="N49" s="1"/>
       <c r="O49" s="2"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -5463,7 +5496,7 @@
       <c r="N50" s="1"/>
       <c r="O50" s="2"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -5476,7 +5509,7 @@
       <c r="N51" s="1"/>
       <c r="O51" s="2"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -5489,7 +5522,7 @@
       <c r="N52" s="1"/>
       <c r="O52" s="2"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -5502,7 +5535,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="2"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -5515,235 +5548,235 @@
       <c r="N54" s="1"/>
       <c r="O54" s="2"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="K107" s="1"/>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="K111" s="1"/>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="K112" s="1"/>
     </row>
@@ -5753,16 +5786,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5773,7 +5806,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -5785,10 +5818,10 @@
         <v>1</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5808,7 +5841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5828,185 +5861,185 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>0.1</v>
+      </c>
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
-        <v>0.1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <f>B6*3.14159/180</f>
         <v>0.13962622222222221</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>8</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6">
         <f>I6*3.14159/180</f>
         <v>0.13962622222222221</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f>B7*3.14159/180</f>
         <v>0.13962622222222221</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7">
         <v>8</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <f>I7*3.14159/180</f>
         <v>0.13962622222222221</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -6054,7 +6087,7 @@
         <v>1.7326797801464373</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>1.2*A10</f>
         <v>6</v>
@@ -6104,7 +6137,7 @@
         <v>1.8376740969126244</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" ref="A12:A52" si="10">1.2*A11</f>
         <v>7.1999999999999993</v>
@@ -6154,7 +6187,7 @@
         <v>2.1351004527180679</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="10"/>
         <v>8.6399999999999988</v>
@@ -6204,7 +6237,7 @@
         <v>2.6458834749500202</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="10"/>
         <v>10.367999999999999</v>
@@ -6254,7 +6287,7 @@
         <v>3.4309633900253602</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="10"/>
         <v>12.441599999999998</v>
@@ -6304,7 +6337,7 @@
         <v>4.5925840495850538</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="10"/>
         <v>14.929919999999996</v>
@@ -6354,7 +6387,7 @@
         <v>6.2854526490276772</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="10"/>
         <v>17.915903999999994</v>
@@ -6404,7 +6437,7 @@
         <v>8.7364988143595816</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="10"/>
         <v>21.499084799999991</v>
@@ -6454,7 +6487,7 @@
         <v>12.274943092030879</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="10"/>
         <v>25.798901759999989</v>
@@ -6504,7 +6537,7 @@
         <v>17.376364769561608</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="10"/>
         <v>30.958682111999984</v>
@@ -6554,7 +6587,7 @@
         <v>24.726553127317821</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="10"/>
         <v>37.150418534399982</v>
@@ -6604,7 +6637,7 @@
         <v>35.313667554863066</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="10"/>
         <v>44.58050224127998</v>
@@ -6654,7 +6687,7 @@
         <v>50.561071195096332</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="10"/>
         <v>53.496602689535976</v>
@@ -6704,7 +6737,7 @@
         <v>72.518685297680634</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="10"/>
         <v>64.195923227443174</v>
@@ -6754,7 +6787,7 @@
         <v>104.13858550970082</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="10"/>
         <v>77.035107872931803</v>
@@ -6804,7 +6837,7 @@
         <v>149.67189002642968</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="10"/>
         <v>92.442129447518155</v>
@@ -6854,23 +6887,23 @@
         <v>215.24029784865647</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="6">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>100</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <f t="shared" si="1"/>
         <v>13.962622222222221</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <f t="shared" si="2"/>
         <v>13.962622222222221</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <f t="shared" si="3"/>
         <v>407.12860060047933</v>
       </c>
@@ -6878,18 +6911,18 @@
         <f t="shared" si="4"/>
         <v>614.05658956720731</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>100</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="5">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="5">
         <f t="shared" si="6"/>
         <v>13.962622222222221</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="5">
         <f t="shared" si="7"/>
         <v>13.962622222222221</v>
       </c>
@@ -6902,7 +6935,7 @@
         <v>251.76320172255498</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="10"/>
         <v>120</v>
@@ -6952,11 +6985,11 @@
         <v>362.25220125744517</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="5">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>300</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -6976,10 +7009,10 @@
         <f t="shared" si="4"/>
         <v>5513.799719788929</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="4">
         <v>300</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="4">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
@@ -7000,7 +7033,7 @@
         <v>2260.6578851134609</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="10"/>
         <v>360</v>
@@ -7050,7 +7083,7 @@
         <v>3255.0610823707589</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="10"/>
         <v>432</v>
@@ -7100,7 +7133,7 @@
         <v>4687.0017069135665</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="10"/>
         <v>518.4</v>
@@ -7150,11 +7183,11 @@
         <v>6748.9962204851417</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="5">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>600</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -7174,10 +7207,10 @@
         <f t="shared" si="4"/>
         <v>22050.438547637219</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="4">
         <v>600</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I33" s="4">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
@@ -7198,7 +7231,7 @@
         <v>9040.6798045312589</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="10"/>
         <v>720</v>
@@ -7248,7 +7281,7 @@
         <v>13018.292696629151</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="10"/>
         <v>864</v>
@@ -7298,7 +7331,7 @@
         <v>18746.055266372441</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1000</v>
       </c>
@@ -7346,7 +7379,7 @@
         <v>25111.843018295738</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="10"/>
         <v>1200</v>
@@ -7396,7 +7429,7 @@
         <v>36160.767735178873</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="10"/>
         <v>1440</v>
@@ -7446,7 +7479,7 @@
         <v>52071.219329334577</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="10"/>
         <v>1728</v>
@@ -7496,11 +7529,11 @@
         <v>74982.269626199282</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="5">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>2000</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -7520,10 +7553,10 @@
         <f t="shared" si="4"/>
         <v>244988.83083951354</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="4">
         <v>2000</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I40" s="4">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
@@ -7544,7 +7577,7 @@
         <v>100445.42064420055</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="10"/>
         <v>2400</v>
@@ -7594,7 +7627,7 @@
         <v>144641.1195210079</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="10"/>
         <v>2880</v>
@@ -7644,7 +7677,7 @@
         <v>208282.92590407163</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="10"/>
         <v>3456</v>
@@ -7694,7 +7727,7 @@
         <v>299927.12709600321</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="10"/>
         <v>4147.2</v>
@@ -7744,7 +7777,7 @@
         <v>431894.77681260725</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="10"/>
         <v>4976.6399999999994</v>
@@ -7794,7 +7827,7 @@
         <v>621928.19240467134</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="10"/>
         <v>5971.9679999999989</v>
@@ -7844,7 +7877,7 @@
         <v>895576.31085735071</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="10"/>
         <v>7166.3615999999984</v>
@@ -7894,7 +7927,7 @@
         <v>1289629.6014292832</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="10"/>
         <v>8599.6339199999984</v>
@@ -7944,7 +7977,7 @@
         <v>1857066.3398529186</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="10"/>
         <v>10319.560703999998</v>
@@ -7994,7 +8027,7 @@
         <v>2674175.2431829888</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="10"/>
         <v>12383.472844799997</v>
@@ -8044,7 +8077,7 @@
         <v>3850812.0639783158</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="10"/>
         <v>14860.167413759995</v>
@@ -8094,7 +8127,7 @@
         <v>5545169.0859236</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="10"/>
         <v>17832.200896511993</v>
@@ -8144,235 +8177,235 @@
         <v>7985043.1975248232</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="H110" s="1"/>
     </row>

</xml_diff>